<commit_message>
Fuck that shit :wink:
</commit_message>
<xml_diff>
--- a/Data/Contacts.xlsx
+++ b/Data/Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8CCE2C-4EBC-4843-891B-EE428FA327D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372CE724-086A-40C1-A82F-4A7951DDA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +206,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -326,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -340,9 +353,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,6 +394,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -675,24 +694,24 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="24" style="6" customWidth="1"/>
-    <col min="4" max="4" width="19" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="22" style="8" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="6" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="6"/>
-    <col min="11" max="11" width="9.140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="6" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="14" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="22" style="7" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="5" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="9.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -702,22 +721,22 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -728,19 +747,19 @@
       <c r="B2" s="4">
         <v>7129</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="4"/>
@@ -752,17 +771,17 @@
       <c r="B3" s="4">
         <v>7379</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="4"/>
@@ -777,19 +796,19 @@
       <c r="B4" s="4">
         <v>7286</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="4"/>
@@ -804,17 +823,17 @@
       <c r="B5" s="4">
         <v>7387</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="16" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="4"/>
@@ -829,17 +848,17 @@
       <c r="B6" s="4">
         <v>7265</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="4"/>
@@ -848,25 +867,25 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="17">
         <v>14000523</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>7265</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="4" t="s">
         <v>38</v>
       </c>
@@ -875,25 +894,25 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="17">
         <v>14000523</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>7265</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="4"/>
       <c r="M8" s="4" t="s">
         <v>22</v>
@@ -906,17 +925,17 @@
       <c r="B9" s="4">
         <v>7265</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,47 +945,47 @@
       <c r="B10" s="4">
         <v>7265</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="9" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="17"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="17"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contact Info Updated :grin:
</commit_message>
<xml_diff>
--- a/Data/Contacts.xlsx
+++ b/Data/Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5396E8-BC48-442D-8DBB-154CE6C2C906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D456EFA-20F9-4B20-B833-CF9633DE3362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>Task</t>
   </si>
@@ -148,6 +148,150 @@
   </si>
   <si>
     <t>09189401186</t>
+  </si>
+  <si>
+    <t>جعفری</t>
+  </si>
+  <si>
+    <t>شمال کرمان</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>09132461348</t>
+  </si>
+  <si>
+    <t>سلطانی</t>
+  </si>
+  <si>
+    <t>034-31251183</t>
+  </si>
+  <si>
+    <t>گیلان</t>
+  </si>
+  <si>
+    <t>013-33571275</t>
+  </si>
+  <si>
+    <t>تبریز</t>
+  </si>
+  <si>
+    <t>قهرمانی</t>
+  </si>
+  <si>
+    <t>09144163794</t>
+  </si>
+  <si>
+    <t>خراسان</t>
+  </si>
+  <si>
+    <t>محمدی</t>
+  </si>
+  <si>
+    <t>09105163424</t>
+  </si>
+  <si>
+    <t>احمدی</t>
+  </si>
+  <si>
+    <t>کردستان</t>
+  </si>
+  <si>
+    <t>09189698389</t>
+  </si>
+  <si>
+    <t>زمانپور</t>
+  </si>
+  <si>
+    <t>بوشهر</t>
+  </si>
+  <si>
+    <t>077-31281008</t>
+  </si>
+  <si>
+    <t>عشرت خواه</t>
+  </si>
+  <si>
+    <t>وحدتی</t>
+  </si>
+  <si>
+    <t>جنوب کرمان</t>
+  </si>
+  <si>
+    <t>034-32116083</t>
+  </si>
+  <si>
+    <t>دهقان</t>
+  </si>
+  <si>
+    <t>یزد</t>
+  </si>
+  <si>
+    <t>09132582328</t>
+  </si>
+  <si>
+    <t>09131964098</t>
+  </si>
+  <si>
+    <t>آذربایجان شرقی</t>
+  </si>
+  <si>
+    <t>یاقوتی</t>
+  </si>
+  <si>
+    <t>09148319202</t>
+  </si>
+  <si>
+    <t>نظامی</t>
+  </si>
+  <si>
+    <t>لرستان</t>
+  </si>
+  <si>
+    <t>09161622355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">محمدی </t>
+  </si>
+  <si>
+    <t>البرز</t>
+  </si>
+  <si>
+    <t>026-32122444</t>
+  </si>
+  <si>
+    <t>حسن دخت</t>
+  </si>
+  <si>
+    <t>09111355532</t>
+  </si>
+  <si>
+    <t>(گیلان)</t>
+  </si>
+  <si>
+    <t>محمود آبادی</t>
+  </si>
+  <si>
+    <t>09131784667</t>
+  </si>
+  <si>
+    <t>عباسی</t>
+  </si>
+  <si>
+    <t>09119928341</t>
+  </si>
+  <si>
+    <t>09114303060</t>
+  </si>
+  <si>
+    <t>آقاجانی</t>
+  </si>
+  <si>
+    <t>دکتر سلطانزاده</t>
+  </si>
+  <si>
+    <t>09112344791</t>
   </si>
 </sst>
 </file>
@@ -272,12 +416,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -354,11 +498,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,22 +565,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -437,10 +584,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -729,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,10 +935,10 @@
       <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="26" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="15" t="s">
@@ -787,10 +952,10 @@
       <c r="B2" s="4">
         <v>7129</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -811,10 +976,10 @@
       <c r="B3" s="4">
         <v>7379</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -836,10 +1001,10 @@
       <c r="B4" s="4">
         <v>7286</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -863,10 +1028,10 @@
       <c r="B5" s="4">
         <v>7387</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -888,10 +1053,10 @@
       <c r="B6" s="4">
         <v>7265</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="12"/>
@@ -907,22 +1072,22 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="28">
         <v>14000523</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="28">
         <v>7265</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="31" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="12"/>
@@ -934,22 +1099,22 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="28">
         <v>14000523</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="28">
         <v>7265</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="31" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="12"/>
@@ -965,10 +1130,10 @@
       <c r="B9" s="4">
         <v>7265</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -977,11 +1142,11 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="4"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
     </row>
     <row r="10" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -990,13 +1155,13 @@
       <c r="B10" s="4">
         <v>7265</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="24" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -1004,81 +1169,443 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="4"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
     </row>
     <row r="11" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="16"/>
+      <c r="A11" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="4"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
     </row>
     <row r="12" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="16"/>
+      <c r="A12" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="27"/>
       <c r="H12" s="4"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
     </row>
     <row r="13" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="16"/>
+      <c r="A13" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="27"/>
       <c r="H13" s="4"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O14" s="23"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+    </row>
+    <row r="14" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="4"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+    </row>
+    <row r="15" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="4"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="22"/>
       <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+    </row>
+    <row r="16" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="4"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="22"/>
       <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+    </row>
+    <row r="17" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="4"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+    </row>
+    <row r="18" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="4"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+    </row>
+    <row r="19" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>14000913</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>14000920</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>14000920</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>14000920</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>14000920</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>14000920</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>14000927</v>
+      </c>
+      <c r="B27" s="4">
+        <v>7486</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>14000927</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>14000927</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>14000927</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6 G11:G13" xr:uid="{2D5B6680-CD00-499F-B74A-D093553486AD}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6 G11:G30" xr:uid="{2D5B6680-CD00-499F-B74A-D093553486AD}">
       <formula1>$M$4:$M$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
ViewServiceLog added for simplicity :grin:
</commit_message>
<xml_diff>
--- a/Data/Contacts.xlsx
+++ b/Data/Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2D50C-3905-4693-A681-1565FB08D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A387150-5515-48E0-A047-733290858C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>Task</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>09188407178</t>
+  </si>
+  <si>
+    <t>09143106803</t>
   </si>
 </sst>
 </file>
@@ -899,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1376,7 @@
         <v>49</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="27"/>

</xml_diff>